<commit_message>
add new results to be analysed
</commit_message>
<xml_diff>
--- a/results/multiple_simulations/obs0.2m/agents5obs0.2.xlsx
+++ b/results/multiple_simulations/obs0.2m/agents5obs0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\Projects\LoadingBots\LoadingBots\results\multiple_simulations\obs0.2m\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512DBA8D-D9ED-4B2A-806A-648F0BE4CAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A6BE7A-30FD-4FB3-AC06-E1EFD2B142BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -337,15 +337,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:U3"/>
+  <dimension ref="B2:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0.31415926535897898</v>
       </c>
@@ -406,8 +406,68 @@
       <c r="U2">
         <v>6.2831853071795898</v>
       </c>
+      <c r="V2">
+        <v>0.31415926535897898</v>
+      </c>
+      <c r="W2">
+        <v>0.62831853071795896</v>
+      </c>
+      <c r="X2">
+        <v>0.94247779607693805</v>
+      </c>
+      <c r="Y2">
+        <v>1.2566370614359199</v>
+      </c>
+      <c r="Z2">
+        <v>1.5707963267949001</v>
+      </c>
+      <c r="AA2">
+        <v>1.8849555921538801</v>
+      </c>
+      <c r="AB2">
+        <v>2.1991148575128601</v>
+      </c>
+      <c r="AC2">
+        <v>2.5132741228718301</v>
+      </c>
+      <c r="AD2">
+        <v>2.8274333882308098</v>
+      </c>
+      <c r="AE2">
+        <v>3.14159265358979</v>
+      </c>
+      <c r="AF2">
+        <v>3.4557519189487702</v>
+      </c>
+      <c r="AG2">
+        <v>3.76991118430775</v>
+      </c>
+      <c r="AH2">
+        <v>4.0840704496667302</v>
+      </c>
+      <c r="AI2">
+        <v>4.3982297150257104</v>
+      </c>
+      <c r="AJ2">
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="AK2">
+        <v>5.0265482457436699</v>
+      </c>
+      <c r="AL2">
+        <v>5.3407075111026501</v>
+      </c>
+      <c r="AM2">
+        <v>5.6548667764616303</v>
+      </c>
+      <c r="AN2">
+        <v>5.9690260418206096</v>
+      </c>
+      <c r="AO2">
+        <v>6.2831853071795898</v>
+      </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -466,6 +526,66 @@
         <v>0</v>
       </c>
       <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3">
         <v>1</v>
       </c>
     </row>

</xml_diff>